<commit_message>
ULTIMA VERSION- VERSION NOTEBOOK TERMINADA- VERSION COMPUTADORA PENDIENTE
</commit_message>
<xml_diff>
--- a/Dulce Azar/AppWeb 5.0 Version_Computadora/Baroque Corporation Análisis/Diagrama de Gantt-Dulce Azar.xlsx
+++ b/Dulce Azar/AppWeb 5.0 Version_Computadora/Baroque Corporation Análisis/Diagrama de Gantt-Dulce Azar.xlsx
@@ -481,7 +481,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="18">
     <border/>
     <border>
       <left style="thick">
@@ -553,7 +553,7 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thick">
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -564,7 +564,7 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thick">
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -578,7 +578,7 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thick">
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -592,7 +592,7 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thick">
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -600,10 +600,69 @@
       <left style="thick">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thin">
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -615,95 +674,6 @@
         <color rgb="FF000000"/>
       </right>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -722,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -752,48 +722,43 @@
     <xf borderId="11" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="9" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="10" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="13" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="13" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf borderId="13" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="13" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="15" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="16" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="17" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="15" fillId="5" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="19" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="19" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="20" fillId="6" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="16" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="6" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="15" fillId="5" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1223,33 +1188,33 @@
       <c r="J4" s="14"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="16"/>
-      <c r="AC4" s="16"/>
-      <c r="AD4" s="16"/>
-      <c r="AE4" s="16"/>
-      <c r="AF4" s="16"/>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="16"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-      <c r="AM4" s="16"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="14"/>
+      <c r="AG4" s="14"/>
+      <c r="AH4" s="14"/>
+      <c r="AI4" s="14"/>
+      <c r="AJ4" s="14"/>
+      <c r="AK4" s="14"/>
+      <c r="AL4" s="14"/>
+      <c r="AM4" s="14"/>
       <c r="AN4" s="16"/>
     </row>
     <row r="5">
@@ -1276,7 +1241,7 @@
         <v>54</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="16"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
@@ -1309,7 +1274,7 @@
       <c r="AN5" s="16"/>
     </row>
     <row r="6">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="13">
@@ -1332,40 +1297,40 @@
         <v>59</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
       <c r="L6" s="15"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="16"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="16"/>
-      <c r="AF6" s="16"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="16"/>
-      <c r="AI6" s="16"/>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="16"/>
-      <c r="AL6" s="16"/>
-      <c r="AM6" s="16"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="14"/>
+      <c r="AH6" s="14"/>
+      <c r="AI6" s="14"/>
+      <c r="AJ6" s="14"/>
+      <c r="AK6" s="14"/>
+      <c r="AL6" s="14"/>
+      <c r="AM6" s="14"/>
       <c r="AN6" s="16"/>
     </row>
     <row r="7">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="13">
@@ -1388,40 +1353,40 @@
         <v>59</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="16"/>
-      <c r="AB7" s="16"/>
-      <c r="AC7" s="16"/>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="16"/>
-      <c r="AF7" s="16"/>
-      <c r="AG7" s="16"/>
-      <c r="AH7" s="16"/>
-      <c r="AI7" s="16"/>
-      <c r="AJ7" s="16"/>
-      <c r="AK7" s="16"/>
-      <c r="AL7" s="16"/>
-      <c r="AM7" s="16"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="14"/>
+      <c r="AF7" s="14"/>
+      <c r="AG7" s="14"/>
+      <c r="AH7" s="14"/>
+      <c r="AI7" s="14"/>
+      <c r="AJ7" s="14"/>
+      <c r="AK7" s="14"/>
+      <c r="AL7" s="14"/>
+      <c r="AM7" s="14"/>
       <c r="AN7" s="16"/>
     </row>
     <row r="8">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="13">
@@ -1444,40 +1409,40 @@
         <v>54</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
       <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="16"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="16"/>
-      <c r="AD8" s="16"/>
-      <c r="AE8" s="16"/>
-      <c r="AF8" s="16"/>
-      <c r="AG8" s="16"/>
-      <c r="AH8" s="16"/>
-      <c r="AI8" s="16"/>
-      <c r="AJ8" s="16"/>
-      <c r="AK8" s="16"/>
-      <c r="AL8" s="16"/>
-      <c r="AM8" s="16"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="14"/>
+      <c r="AG8" s="14"/>
+      <c r="AH8" s="14"/>
+      <c r="AI8" s="14"/>
+      <c r="AJ8" s="14"/>
+      <c r="AK8" s="14"/>
+      <c r="AL8" s="14"/>
+      <c r="AM8" s="14"/>
       <c r="AN8" s="16"/>
     </row>
     <row r="9">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C9" s="13">
@@ -1487,53 +1452,53 @@
       <c r="D9" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="13">
         <v>15.0</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
       <c r="M9" s="15"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="16"/>
-      <c r="AC9" s="16"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="16"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="16"/>
-      <c r="AI9" s="16"/>
-      <c r="AJ9" s="16"/>
-      <c r="AK9" s="16"/>
-      <c r="AL9" s="16"/>
-      <c r="AM9" s="16"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+      <c r="AH9" s="14"/>
+      <c r="AI9" s="14"/>
+      <c r="AJ9" s="14"/>
+      <c r="AK9" s="14"/>
+      <c r="AL9" s="14"/>
+      <c r="AM9" s="14"/>
       <c r="AN9" s="16"/>
     </row>
     <row r="10">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C10" s="13">
@@ -1543,55 +1508,55 @@
       <c r="D10" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="13">
         <v>15.0</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14" t="s">
         <v>68</v>
       </c>
       <c r="M10" s="15"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="16"/>
-      <c r="AC10" s="16"/>
-      <c r="AD10" s="16"/>
-      <c r="AE10" s="16"/>
-      <c r="AF10" s="16"/>
-      <c r="AG10" s="16"/>
-      <c r="AH10" s="16"/>
-      <c r="AI10" s="16"/>
-      <c r="AJ10" s="16"/>
-      <c r="AK10" s="16"/>
-      <c r="AL10" s="16"/>
-      <c r="AM10" s="16"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="14"/>
+      <c r="AB10" s="14"/>
+      <c r="AC10" s="14"/>
+      <c r="AD10" s="14"/>
+      <c r="AE10" s="14"/>
+      <c r="AF10" s="14"/>
+      <c r="AG10" s="14"/>
+      <c r="AH10" s="14"/>
+      <c r="AI10" s="14"/>
+      <c r="AJ10" s="14"/>
+      <c r="AK10" s="14"/>
+      <c r="AL10" s="14"/>
+      <c r="AM10" s="14"/>
       <c r="AN10" s="16"/>
     </row>
     <row r="11">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="13">
@@ -1601,53 +1566,53 @@
       <c r="D11" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="13">
         <v>15.0</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
       <c r="M11" s="15"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="16"/>
-      <c r="AC11" s="16"/>
-      <c r="AD11" s="16"/>
-      <c r="AE11" s="16"/>
-      <c r="AF11" s="16"/>
-      <c r="AG11" s="16"/>
-      <c r="AH11" s="16"/>
-      <c r="AI11" s="16"/>
-      <c r="AJ11" s="16"/>
-      <c r="AK11" s="16"/>
-      <c r="AL11" s="16"/>
-      <c r="AM11" s="16"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="14"/>
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="14"/>
+      <c r="AG11" s="14"/>
+      <c r="AH11" s="14"/>
+      <c r="AI11" s="14"/>
+      <c r="AJ11" s="14"/>
+      <c r="AK11" s="14"/>
+      <c r="AL11" s="14"/>
+      <c r="AM11" s="14"/>
       <c r="AN11" s="16"/>
     </row>
     <row r="12">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="13">
@@ -1666,51 +1631,51 @@
       <c r="G12" s="13">
         <v>15.0</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
       <c r="M12" s="15"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="16"/>
-      <c r="AA12" s="16"/>
-      <c r="AB12" s="16"/>
-      <c r="AC12" s="16"/>
-      <c r="AD12" s="16"/>
-      <c r="AE12" s="16"/>
-      <c r="AF12" s="16"/>
-      <c r="AG12" s="16"/>
-      <c r="AH12" s="16"/>
-      <c r="AI12" s="16"/>
-      <c r="AJ12" s="16"/>
-      <c r="AK12" s="16"/>
-      <c r="AL12" s="16"/>
-      <c r="AM12" s="16"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="14"/>
+      <c r="AE12" s="14"/>
+      <c r="AF12" s="14"/>
+      <c r="AG12" s="14"/>
+      <c r="AH12" s="14"/>
+      <c r="AI12" s="14"/>
+      <c r="AJ12" s="14"/>
+      <c r="AK12" s="14"/>
+      <c r="AL12" s="14"/>
+      <c r="AM12" s="14"/>
       <c r="AN12" s="16"/>
     </row>
     <row r="13">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="13">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="13" t="s">
         <v>72</v>
       </c>
       <c r="E13" s="13" t="s">
@@ -1722,51 +1687,51 @@
       <c r="G13" s="13">
         <v>25.0</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
       <c r="N13" s="15"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="16"/>
-      <c r="AA13" s="16"/>
-      <c r="AB13" s="16"/>
-      <c r="AC13" s="16"/>
-      <c r="AD13" s="16"/>
-      <c r="AE13" s="16"/>
-      <c r="AF13" s="16"/>
-      <c r="AG13" s="16"/>
-      <c r="AH13" s="16"/>
-      <c r="AI13" s="16"/>
-      <c r="AJ13" s="16"/>
-      <c r="AK13" s="16"/>
-      <c r="AL13" s="16"/>
-      <c r="AM13" s="16"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="14"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="14"/>
+      <c r="AG13" s="14"/>
+      <c r="AH13" s="14"/>
+      <c r="AI13" s="14"/>
+      <c r="AJ13" s="14"/>
+      <c r="AK13" s="14"/>
+      <c r="AL13" s="14"/>
+      <c r="AM13" s="14"/>
       <c r="AN13" s="16"/>
     </row>
     <row r="14">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C14" s="13">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="13" t="s">
         <v>73</v>
       </c>
       <c r="E14" s="13" t="s">
@@ -1778,51 +1743,51 @@
       <c r="G14" s="13">
         <v>25.0</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
       <c r="N14" s="15"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="16"/>
-      <c r="V14" s="16"/>
-      <c r="W14" s="16"/>
-      <c r="X14" s="16"/>
-      <c r="Y14" s="16"/>
-      <c r="Z14" s="16"/>
-      <c r="AA14" s="16"/>
-      <c r="AB14" s="16"/>
-      <c r="AC14" s="16"/>
-      <c r="AD14" s="16"/>
-      <c r="AE14" s="16"/>
-      <c r="AF14" s="16"/>
-      <c r="AG14" s="16"/>
-      <c r="AH14" s="16"/>
-      <c r="AI14" s="16"/>
-      <c r="AJ14" s="16"/>
-      <c r="AK14" s="16"/>
-      <c r="AL14" s="16"/>
-      <c r="AM14" s="16"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
+      <c r="AG14" s="14"/>
+      <c r="AH14" s="14"/>
+      <c r="AI14" s="14"/>
+      <c r="AJ14" s="14"/>
+      <c r="AK14" s="14"/>
+      <c r="AL14" s="14"/>
+      <c r="AM14" s="14"/>
       <c r="AN14" s="16"/>
     </row>
     <row r="15">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C15" s="13">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="13" t="s">
         <v>74</v>
       </c>
       <c r="E15" s="13" t="s">
@@ -1834,51 +1799,51 @@
       <c r="G15" s="13">
         <v>25.0</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
       <c r="N15" s="15"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="16"/>
-      <c r="X15" s="16"/>
-      <c r="Y15" s="16"/>
-      <c r="Z15" s="16"/>
-      <c r="AA15" s="16"/>
-      <c r="AB15" s="16"/>
-      <c r="AC15" s="16"/>
-      <c r="AD15" s="16"/>
-      <c r="AE15" s="16"/>
-      <c r="AF15" s="16"/>
-      <c r="AG15" s="16"/>
-      <c r="AH15" s="16"/>
-      <c r="AI15" s="16"/>
-      <c r="AJ15" s="16"/>
-      <c r="AK15" s="16"/>
-      <c r="AL15" s="16"/>
-      <c r="AM15" s="16"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="14"/>
+      <c r="AE15" s="14"/>
+      <c r="AF15" s="14"/>
+      <c r="AG15" s="14"/>
+      <c r="AH15" s="14"/>
+      <c r="AI15" s="14"/>
+      <c r="AJ15" s="14"/>
+      <c r="AK15" s="14"/>
+      <c r="AL15" s="14"/>
+      <c r="AM15" s="14"/>
       <c r="AN15" s="16"/>
     </row>
     <row r="16">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C16" s="13">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="13" t="s">
         <v>75</v>
       </c>
       <c r="E16" s="13" t="s">
@@ -1890,51 +1855,51 @@
       <c r="G16" s="13">
         <v>25.0</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
       <c r="N16" s="15"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="16"/>
-      <c r="X16" s="16"/>
-      <c r="Y16" s="16"/>
-      <c r="Z16" s="16"/>
-      <c r="AA16" s="16"/>
-      <c r="AB16" s="16"/>
-      <c r="AC16" s="16"/>
-      <c r="AD16" s="16"/>
-      <c r="AE16" s="16"/>
-      <c r="AF16" s="16"/>
-      <c r="AG16" s="16"/>
-      <c r="AH16" s="16"/>
-      <c r="AI16" s="16"/>
-      <c r="AJ16" s="16"/>
-      <c r="AK16" s="16"/>
-      <c r="AL16" s="16"/>
-      <c r="AM16" s="16"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="14"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="14"/>
+      <c r="AE16" s="14"/>
+      <c r="AF16" s="14"/>
+      <c r="AG16" s="14"/>
+      <c r="AH16" s="14"/>
+      <c r="AI16" s="14"/>
+      <c r="AJ16" s="14"/>
+      <c r="AK16" s="14"/>
+      <c r="AL16" s="14"/>
+      <c r="AM16" s="14"/>
       <c r="AN16" s="16"/>
     </row>
     <row r="17">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="13">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="13" t="s">
         <v>76</v>
       </c>
       <c r="E17" s="13" t="s">
@@ -1946,291 +1911,291 @@
       <c r="G17" s="13">
         <v>25.0</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
       <c r="N17" s="15"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="16"/>
-      <c r="Y17" s="16"/>
-      <c r="Z17" s="16"/>
-      <c r="AA17" s="16"/>
-      <c r="AB17" s="16"/>
-      <c r="AC17" s="16"/>
-      <c r="AD17" s="16"/>
-      <c r="AE17" s="16"/>
-      <c r="AF17" s="16"/>
-      <c r="AG17" s="16"/>
-      <c r="AH17" s="16"/>
-      <c r="AI17" s="16"/>
-      <c r="AJ17" s="16"/>
-      <c r="AK17" s="16"/>
-      <c r="AL17" s="16"/>
-      <c r="AM17" s="16"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="14"/>
+      <c r="X17" s="14"/>
+      <c r="Y17" s="14"/>
+      <c r="Z17" s="14"/>
+      <c r="AA17" s="14"/>
+      <c r="AB17" s="14"/>
+      <c r="AC17" s="14"/>
+      <c r="AD17" s="14"/>
+      <c r="AE17" s="14"/>
+      <c r="AF17" s="14"/>
+      <c r="AG17" s="14"/>
+      <c r="AH17" s="14"/>
+      <c r="AI17" s="14"/>
+      <c r="AJ17" s="14"/>
+      <c r="AK17" s="14"/>
+      <c r="AL17" s="14"/>
+      <c r="AM17" s="14"/>
       <c r="AN17" s="16"/>
     </row>
     <row r="18">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C18" s="13">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="13">
         <v>17.0</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
       <c r="N18" s="15"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-      <c r="X18" s="16"/>
-      <c r="Y18" s="16"/>
-      <c r="Z18" s="16"/>
-      <c r="AA18" s="16"/>
-      <c r="AB18" s="16"/>
-      <c r="AC18" s="16"/>
-      <c r="AD18" s="16"/>
-      <c r="AE18" s="16"/>
-      <c r="AF18" s="16"/>
-      <c r="AG18" s="16"/>
-      <c r="AH18" s="16"/>
-      <c r="AI18" s="16"/>
-      <c r="AJ18" s="16"/>
-      <c r="AK18" s="16"/>
-      <c r="AL18" s="16"/>
-      <c r="AM18" s="16"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="14"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="14"/>
+      <c r="AG18" s="14"/>
+      <c r="AH18" s="14"/>
+      <c r="AI18" s="14"/>
+      <c r="AJ18" s="14"/>
+      <c r="AK18" s="14"/>
+      <c r="AL18" s="14"/>
+      <c r="AM18" s="14"/>
       <c r="AN18" s="16"/>
     </row>
     <row r="19">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="13">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="13">
         <v>18.0</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
       <c r="N19" s="15"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="16"/>
-      <c r="V19" s="16"/>
-      <c r="W19" s="16"/>
-      <c r="X19" s="16"/>
-      <c r="Y19" s="16"/>
-      <c r="Z19" s="16"/>
-      <c r="AA19" s="16"/>
-      <c r="AB19" s="16"/>
-      <c r="AC19" s="16"/>
-      <c r="AD19" s="16"/>
-      <c r="AE19" s="16"/>
-      <c r="AF19" s="16"/>
-      <c r="AG19" s="16"/>
-      <c r="AH19" s="16"/>
-      <c r="AI19" s="16"/>
-      <c r="AJ19" s="16"/>
-      <c r="AK19" s="16"/>
-      <c r="AL19" s="16"/>
-      <c r="AM19" s="16"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="14"/>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="14"/>
+      <c r="Z19" s="14"/>
+      <c r="AA19" s="14"/>
+      <c r="AB19" s="14"/>
+      <c r="AC19" s="14"/>
+      <c r="AD19" s="14"/>
+      <c r="AE19" s="14"/>
+      <c r="AF19" s="14"/>
+      <c r="AG19" s="14"/>
+      <c r="AH19" s="14"/>
+      <c r="AI19" s="14"/>
+      <c r="AJ19" s="14"/>
+      <c r="AK19" s="14"/>
+      <c r="AL19" s="14"/>
+      <c r="AM19" s="14"/>
       <c r="AN19" s="16"/>
     </row>
     <row r="20">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C20" s="13">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="13">
         <v>15.0</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="13">
         <v>23.0</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
       <c r="N20" s="15"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="16"/>
-      <c r="X20" s="16"/>
-      <c r="Y20" s="16"/>
-      <c r="Z20" s="16"/>
-      <c r="AA20" s="16"/>
-      <c r="AB20" s="16"/>
-      <c r="AC20" s="16"/>
-      <c r="AD20" s="16"/>
-      <c r="AE20" s="16"/>
-      <c r="AF20" s="16"/>
-      <c r="AG20" s="16"/>
-      <c r="AH20" s="16"/>
-      <c r="AI20" s="16"/>
-      <c r="AJ20" s="16"/>
-      <c r="AK20" s="16"/>
-      <c r="AL20" s="16"/>
-      <c r="AM20" s="16"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="14"/>
+      <c r="AA20" s="14"/>
+      <c r="AB20" s="14"/>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="14"/>
+      <c r="AE20" s="14"/>
+      <c r="AF20" s="14"/>
+      <c r="AG20" s="14"/>
+      <c r="AH20" s="14"/>
+      <c r="AI20" s="14"/>
+      <c r="AJ20" s="14"/>
+      <c r="AK20" s="14"/>
+      <c r="AL20" s="14"/>
+      <c r="AM20" s="14"/>
       <c r="AN20" s="16"/>
     </row>
     <row r="21">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C21" s="13">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="13">
         <v>16.0</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="13">
         <v>23.0</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
       <c r="N21" s="15"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="16"/>
-      <c r="Z21" s="16"/>
-      <c r="AA21" s="16"/>
-      <c r="AB21" s="16"/>
-      <c r="AC21" s="16"/>
-      <c r="AD21" s="16"/>
-      <c r="AE21" s="16"/>
-      <c r="AF21" s="16"/>
-      <c r="AG21" s="16"/>
-      <c r="AH21" s="16"/>
-      <c r="AI21" s="16"/>
-      <c r="AJ21" s="16"/>
-      <c r="AK21" s="16"/>
-      <c r="AL21" s="16"/>
-      <c r="AM21" s="16"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="14"/>
+      <c r="X21" s="14"/>
+      <c r="Y21" s="14"/>
+      <c r="Z21" s="14"/>
+      <c r="AA21" s="14"/>
+      <c r="AB21" s="14"/>
+      <c r="AC21" s="14"/>
+      <c r="AD21" s="14"/>
+      <c r="AE21" s="14"/>
+      <c r="AF21" s="14"/>
+      <c r="AG21" s="14"/>
+      <c r="AH21" s="14"/>
+      <c r="AI21" s="14"/>
+      <c r="AJ21" s="14"/>
+      <c r="AK21" s="14"/>
+      <c r="AL21" s="14"/>
+      <c r="AM21" s="14"/>
       <c r="AN21" s="16"/>
     </row>
     <row r="22">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="12" t="s">
         <v>84</v>
       </c>
       <c r="C22" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="13">
         <v>18.0</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="13">
         <v>20.0</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
@@ -2238,279 +2203,279 @@
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
-      <c r="R22" s="16"/>
-      <c r="S22" s="16"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="16"/>
-      <c r="W22" s="16"/>
-      <c r="X22" s="16"/>
-      <c r="Y22" s="16"/>
-      <c r="Z22" s="16"/>
-      <c r="AA22" s="16"/>
-      <c r="AB22" s="16"/>
-      <c r="AC22" s="16"/>
-      <c r="AD22" s="16"/>
-      <c r="AE22" s="16"/>
-      <c r="AF22" s="16"/>
-      <c r="AG22" s="16"/>
-      <c r="AH22" s="16"/>
-      <c r="AI22" s="16"/>
-      <c r="AJ22" s="16"/>
-      <c r="AK22" s="16"/>
-      <c r="AL22" s="16"/>
-      <c r="AM22" s="16"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="14"/>
+      <c r="W22" s="14"/>
+      <c r="X22" s="14"/>
+      <c r="Y22" s="14"/>
+      <c r="Z22" s="14"/>
+      <c r="AA22" s="14"/>
+      <c r="AB22" s="14"/>
+      <c r="AC22" s="14"/>
+      <c r="AD22" s="14"/>
+      <c r="AE22" s="14"/>
+      <c r="AF22" s="14"/>
+      <c r="AG22" s="14"/>
+      <c r="AH22" s="14"/>
+      <c r="AI22" s="14"/>
+      <c r="AJ22" s="14"/>
+      <c r="AK22" s="14"/>
+      <c r="AL22" s="14"/>
+      <c r="AM22" s="14"/>
       <c r="AN22" s="16"/>
     </row>
     <row r="23">
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="12" t="s">
         <v>86</v>
       </c>
       <c r="C23" s="13">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="13">
         <v>20.0</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="16"/>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="16"/>
-      <c r="Z23" s="16"/>
-      <c r="AA23" s="16"/>
-      <c r="AB23" s="16"/>
-      <c r="AC23" s="16"/>
-      <c r="AD23" s="16"/>
-      <c r="AE23" s="16"/>
-      <c r="AF23" s="16"/>
-      <c r="AG23" s="16"/>
-      <c r="AH23" s="16"/>
-      <c r="AI23" s="16"/>
-      <c r="AJ23" s="16"/>
-      <c r="AK23" s="16"/>
-      <c r="AL23" s="16"/>
-      <c r="AM23" s="16"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="14"/>
+      <c r="X23" s="14"/>
+      <c r="Y23" s="14"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="14"/>
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="14"/>
+      <c r="AD23" s="14"/>
+      <c r="AE23" s="14"/>
+      <c r="AF23" s="14"/>
+      <c r="AG23" s="14"/>
+      <c r="AH23" s="14"/>
+      <c r="AI23" s="14"/>
+      <c r="AJ23" s="14"/>
+      <c r="AK23" s="14"/>
+      <c r="AL23" s="14"/>
+      <c r="AM23" s="14"/>
       <c r="AN23" s="16"/>
     </row>
     <row r="24">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="12" t="s">
         <v>89</v>
       </c>
       <c r="C24" s="13">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="13">
         <v>19.0</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="13">
         <v>23.0</v>
       </c>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
-      <c r="U24" s="16"/>
-      <c r="V24" s="16"/>
-      <c r="W24" s="16"/>
-      <c r="X24" s="16"/>
-      <c r="Y24" s="16"/>
-      <c r="Z24" s="16"/>
-      <c r="AA24" s="16"/>
-      <c r="AB24" s="16"/>
-      <c r="AC24" s="16"/>
-      <c r="AD24" s="16"/>
-      <c r="AE24" s="16"/>
-      <c r="AF24" s="16"/>
-      <c r="AG24" s="16"/>
-      <c r="AH24" s="16"/>
-      <c r="AI24" s="16"/>
-      <c r="AJ24" s="16"/>
-      <c r="AK24" s="16"/>
-      <c r="AL24" s="16"/>
-      <c r="AM24" s="16"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="14"/>
+      <c r="W24" s="14"/>
+      <c r="X24" s="14"/>
+      <c r="Y24" s="14"/>
+      <c r="Z24" s="14"/>
+      <c r="AA24" s="14"/>
+      <c r="AB24" s="14"/>
+      <c r="AC24" s="14"/>
+      <c r="AD24" s="14"/>
+      <c r="AE24" s="14"/>
+      <c r="AF24" s="14"/>
+      <c r="AG24" s="14"/>
+      <c r="AH24" s="14"/>
+      <c r="AI24" s="14"/>
+      <c r="AJ24" s="14"/>
+      <c r="AK24" s="14"/>
+      <c r="AL24" s="14"/>
+      <c r="AM24" s="14"/>
       <c r="AN24" s="16"/>
     </row>
     <row r="25">
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="12" t="s">
         <v>91</v>
       </c>
       <c r="C25" s="13">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="13">
         <v>19.0</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="13">
         <v>23.0</v>
       </c>
-      <c r="H25" s="19" t="s">
+      <c r="H25" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
-      <c r="S25" s="16"/>
-      <c r="T25" s="16"/>
-      <c r="U25" s="16"/>
-      <c r="V25" s="16"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="16"/>
-      <c r="Y25" s="16"/>
-      <c r="Z25" s="16"/>
-      <c r="AA25" s="16"/>
-      <c r="AB25" s="16"/>
-      <c r="AC25" s="16"/>
-      <c r="AD25" s="16"/>
-      <c r="AE25" s="16"/>
-      <c r="AF25" s="16"/>
-      <c r="AG25" s="16"/>
-      <c r="AH25" s="16"/>
-      <c r="AI25" s="16"/>
-      <c r="AJ25" s="16"/>
-      <c r="AK25" s="16"/>
-      <c r="AL25" s="16"/>
-      <c r="AM25" s="16"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="14"/>
+      <c r="V25" s="14"/>
+      <c r="W25" s="14"/>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="14"/>
+      <c r="Z25" s="14"/>
+      <c r="AA25" s="14"/>
+      <c r="AB25" s="14"/>
+      <c r="AC25" s="14"/>
+      <c r="AD25" s="14"/>
+      <c r="AE25" s="14"/>
+      <c r="AF25" s="14"/>
+      <c r="AG25" s="14"/>
+      <c r="AH25" s="14"/>
+      <c r="AI25" s="14"/>
+      <c r="AJ25" s="14"/>
+      <c r="AK25" s="14"/>
+      <c r="AL25" s="14"/>
+      <c r="AM25" s="14"/>
       <c r="AN25" s="16"/>
     </row>
     <row r="26">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="13">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="13">
         <v>22.0</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="13">
         <v>24.0</v>
       </c>
-      <c r="H26" s="19" t="s">
+      <c r="H26" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="16"/>
-      <c r="Y26" s="16"/>
-      <c r="Z26" s="16"/>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="16"/>
-      <c r="AC26" s="16"/>
-      <c r="AD26" s="16"/>
-      <c r="AE26" s="16"/>
-      <c r="AF26" s="16"/>
-      <c r="AG26" s="16"/>
-      <c r="AH26" s="16"/>
-      <c r="AI26" s="16"/>
-      <c r="AJ26" s="16"/>
-      <c r="AK26" s="16"/>
-      <c r="AL26" s="16"/>
-      <c r="AM26" s="16"/>
+      <c r="U26" s="14"/>
+      <c r="V26" s="14"/>
+      <c r="W26" s="14"/>
+      <c r="X26" s="14"/>
+      <c r="Y26" s="14"/>
+      <c r="Z26" s="14"/>
+      <c r="AA26" s="14"/>
+      <c r="AB26" s="14"/>
+      <c r="AC26" s="14"/>
+      <c r="AD26" s="14"/>
+      <c r="AE26" s="14"/>
+      <c r="AF26" s="14"/>
+      <c r="AG26" s="14"/>
+      <c r="AH26" s="14"/>
+      <c r="AI26" s="14"/>
+      <c r="AJ26" s="14"/>
+      <c r="AK26" s="14"/>
+      <c r="AL26" s="14"/>
+      <c r="AM26" s="14"/>
       <c r="AN26" s="16"/>
     </row>
     <row r="27">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="12" t="s">
         <v>95</v>
       </c>
       <c r="C27" s="13">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F27" s="13">
         <v>23.0</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="13">
         <v>26.0</v>
       </c>
-      <c r="H27" s="19" t="s">
+      <c r="H27" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
       <c r="M27" s="14"/>
@@ -2523,50 +2488,50 @@
       <c r="T27" s="15"/>
       <c r="U27" s="14"/>
       <c r="V27" s="14"/>
-      <c r="W27" s="16"/>
-      <c r="X27" s="16"/>
-      <c r="Y27" s="16"/>
-      <c r="Z27" s="16"/>
-      <c r="AA27" s="16"/>
-      <c r="AB27" s="16"/>
-      <c r="AC27" s="16"/>
-      <c r="AD27" s="16"/>
-      <c r="AE27" s="16"/>
-      <c r="AF27" s="16"/>
-      <c r="AG27" s="16"/>
-      <c r="AH27" s="16"/>
-      <c r="AI27" s="16"/>
-      <c r="AJ27" s="16"/>
-      <c r="AK27" s="16"/>
-      <c r="AL27" s="16"/>
-      <c r="AM27" s="16"/>
+      <c r="W27" s="14"/>
+      <c r="X27" s="14"/>
+      <c r="Y27" s="14"/>
+      <c r="Z27" s="14"/>
+      <c r="AA27" s="14"/>
+      <c r="AB27" s="14"/>
+      <c r="AC27" s="14"/>
+      <c r="AD27" s="14"/>
+      <c r="AE27" s="14"/>
+      <c r="AF27" s="14"/>
+      <c r="AG27" s="14"/>
+      <c r="AH27" s="14"/>
+      <c r="AI27" s="14"/>
+      <c r="AJ27" s="14"/>
+      <c r="AK27" s="14"/>
+      <c r="AL27" s="14"/>
+      <c r="AM27" s="14"/>
       <c r="AN27" s="16"/>
     </row>
     <row r="28">
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C28" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="13">
         <v>25.0</v>
       </c>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
@@ -2581,173 +2546,173 @@
       <c r="V28" s="15"/>
       <c r="W28" s="15"/>
       <c r="X28" s="15"/>
-      <c r="Y28" s="16"/>
-      <c r="Z28" s="16"/>
-      <c r="AA28" s="16"/>
-      <c r="AB28" s="16"/>
-      <c r="AC28" s="16"/>
-      <c r="AD28" s="16"/>
-      <c r="AE28" s="16"/>
-      <c r="AF28" s="16"/>
-      <c r="AG28" s="16"/>
-      <c r="AH28" s="16"/>
-      <c r="AI28" s="16"/>
-      <c r="AJ28" s="16"/>
-      <c r="AK28" s="16"/>
-      <c r="AL28" s="16"/>
-      <c r="AM28" s="16"/>
+      <c r="Y28" s="14"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="14"/>
+      <c r="AB28" s="14"/>
+      <c r="AC28" s="14"/>
+      <c r="AD28" s="14"/>
+      <c r="AE28" s="14"/>
+      <c r="AF28" s="14"/>
+      <c r="AG28" s="14"/>
+      <c r="AH28" s="14"/>
+      <c r="AI28" s="14"/>
+      <c r="AJ28" s="14"/>
+      <c r="AK28" s="14"/>
+      <c r="AL28" s="14"/>
+      <c r="AM28" s="14"/>
       <c r="AN28" s="16"/>
     </row>
     <row r="29">
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C29" s="13">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="13">
         <v>26.0</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="16"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="14"/>
+      <c r="T29" s="14"/>
+      <c r="U29" s="14"/>
+      <c r="V29" s="14"/>
+      <c r="W29" s="14"/>
       <c r="X29" s="15"/>
       <c r="Y29" s="15"/>
-      <c r="Z29" s="16"/>
-      <c r="AA29" s="16"/>
-      <c r="AB29" s="16"/>
-      <c r="AC29" s="16"/>
-      <c r="AD29" s="16"/>
-      <c r="AE29" s="16"/>
-      <c r="AF29" s="16"/>
-      <c r="AG29" s="16"/>
-      <c r="AH29" s="16"/>
-      <c r="AI29" s="16"/>
-      <c r="AJ29" s="16"/>
-      <c r="AK29" s="16"/>
-      <c r="AL29" s="16"/>
-      <c r="AM29" s="16"/>
+      <c r="Z29" s="14"/>
+      <c r="AA29" s="14"/>
+      <c r="AB29" s="14"/>
+      <c r="AC29" s="14"/>
+      <c r="AD29" s="14"/>
+      <c r="AE29" s="14"/>
+      <c r="AF29" s="14"/>
+      <c r="AG29" s="14"/>
+      <c r="AH29" s="14"/>
+      <c r="AI29" s="14"/>
+      <c r="AJ29" s="14"/>
+      <c r="AK29" s="14"/>
+      <c r="AL29" s="14"/>
+      <c r="AM29" s="14"/>
       <c r="AN29" s="16"/>
     </row>
     <row r="30">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C30" s="13">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="13">
         <v>28.0</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="13">
         <v>27.0</v>
       </c>
-      <c r="H30" s="19" t="s">
+      <c r="H30" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="16"/>
-      <c r="W30" s="16"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="14"/>
+      <c r="U30" s="14"/>
+      <c r="V30" s="14"/>
+      <c r="W30" s="14"/>
       <c r="X30" s="15"/>
       <c r="Y30" s="15"/>
-      <c r="Z30" s="16"/>
-      <c r="AA30" s="16"/>
-      <c r="AB30" s="16"/>
-      <c r="AC30" s="16"/>
-      <c r="AD30" s="16"/>
-      <c r="AE30" s="16"/>
-      <c r="AF30" s="16"/>
-      <c r="AG30" s="16"/>
-      <c r="AH30" s="16"/>
-      <c r="AI30" s="16"/>
-      <c r="AJ30" s="16"/>
-      <c r="AK30" s="16"/>
-      <c r="AL30" s="16"/>
-      <c r="AM30" s="16"/>
+      <c r="Z30" s="14"/>
+      <c r="AA30" s="14"/>
+      <c r="AB30" s="14"/>
+      <c r="AC30" s="14"/>
+      <c r="AD30" s="14"/>
+      <c r="AE30" s="14"/>
+      <c r="AF30" s="14"/>
+      <c r="AG30" s="14"/>
+      <c r="AH30" s="14"/>
+      <c r="AI30" s="14"/>
+      <c r="AJ30" s="14"/>
+      <c r="AK30" s="14"/>
+      <c r="AL30" s="14"/>
+      <c r="AM30" s="14"/>
       <c r="AN30" s="16"/>
     </row>
     <row r="31">
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C31" s="13">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F31" s="19">
+      <c r="F31" s="13">
         <v>29.0</v>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="13">
         <v>28.0</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H31" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="16"/>
-      <c r="T31" s="16"/>
-      <c r="U31" s="16"/>
-      <c r="V31" s="16"/>
-      <c r="W31" s="16"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="14"/>
+      <c r="W31" s="14"/>
       <c r="X31" s="15"/>
       <c r="Y31" s="15"/>
       <c r="Z31" s="15"/>
@@ -2762,104 +2727,104 @@
       <c r="AI31" s="15"/>
       <c r="AJ31" s="15"/>
       <c r="AK31" s="15"/>
-      <c r="AL31" s="16"/>
-      <c r="AM31" s="16"/>
+      <c r="AL31" s="14"/>
+      <c r="AM31" s="14"/>
       <c r="AN31" s="16"/>
     </row>
     <row r="32">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C32" s="13">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F32" s="13">
         <v>30.0</v>
       </c>
-      <c r="G32" s="19">
+      <c r="G32" s="13">
         <v>29.0</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16"/>
-      <c r="U32" s="16"/>
-      <c r="V32" s="16"/>
-      <c r="W32" s="16"/>
-      <c r="X32" s="22"/>
-      <c r="Y32" s="16"/>
-      <c r="Z32" s="16"/>
-      <c r="AA32" s="16"/>
-      <c r="AB32" s="16"/>
-      <c r="AC32" s="16"/>
-      <c r="AD32" s="16"/>
-      <c r="AE32" s="16"/>
-      <c r="AF32" s="16"/>
-      <c r="AG32" s="16"/>
-      <c r="AH32" s="16"/>
-      <c r="AI32" s="16"/>
-      <c r="AJ32" s="16"/>
-      <c r="AK32" s="16"/>
-      <c r="AL32" s="16"/>
-      <c r="AM32" s="16"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="14"/>
+      <c r="U32" s="14"/>
+      <c r="V32" s="14"/>
+      <c r="W32" s="14"/>
+      <c r="X32" s="19"/>
+      <c r="Y32" s="14"/>
+      <c r="Z32" s="14"/>
+      <c r="AA32" s="14"/>
+      <c r="AB32" s="14"/>
+      <c r="AC32" s="14"/>
+      <c r="AD32" s="14"/>
+      <c r="AE32" s="14"/>
+      <c r="AF32" s="14"/>
+      <c r="AG32" s="14"/>
+      <c r="AH32" s="14"/>
+      <c r="AI32" s="14"/>
+      <c r="AJ32" s="14"/>
+      <c r="AK32" s="14"/>
+      <c r="AL32" s="14"/>
+      <c r="AM32" s="14"/>
       <c r="AN32" s="16"/>
     </row>
     <row r="33">
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C33" s="13">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F33" s="19">
+      <c r="F33" s="13">
         <v>31.0</v>
       </c>
-      <c r="G33" s="19">
+      <c r="G33" s="13">
         <v>30.0</v>
       </c>
-      <c r="H33" s="19" t="s">
+      <c r="H33" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="16"/>
-      <c r="U33" s="16"/>
-      <c r="V33" s="16"/>
-      <c r="W33" s="16"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="14"/>
+      <c r="U33" s="14"/>
+      <c r="V33" s="14"/>
+      <c r="W33" s="14"/>
       <c r="X33" s="15"/>
       <c r="Y33" s="15"/>
       <c r="Z33" s="15"/>
@@ -2874,48 +2839,48 @@
       <c r="AI33" s="15"/>
       <c r="AJ33" s="15"/>
       <c r="AK33" s="15"/>
-      <c r="AL33" s="16"/>
-      <c r="AM33" s="16"/>
+      <c r="AL33" s="14"/>
+      <c r="AM33" s="14"/>
       <c r="AN33" s="16"/>
     </row>
     <row r="34">
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C34" s="13">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F34" s="13">
         <v>32.0</v>
       </c>
-      <c r="G34" s="19">
+      <c r="G34" s="13">
         <v>31.0</v>
       </c>
-      <c r="H34" s="19" t="s">
+      <c r="H34" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="16"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="16"/>
-      <c r="T34" s="16"/>
-      <c r="U34" s="16"/>
-      <c r="V34" s="16"/>
-      <c r="W34" s="16"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="14"/>
+      <c r="V34" s="14"/>
+      <c r="W34" s="14"/>
       <c r="X34" s="15"/>
       <c r="Y34" s="15"/>
       <c r="Z34" s="15"/>
@@ -2923,55 +2888,55 @@
       <c r="AB34" s="15"/>
       <c r="AC34" s="15"/>
       <c r="AD34" s="15"/>
-      <c r="AE34" s="16"/>
-      <c r="AF34" s="16"/>
-      <c r="AG34" s="16"/>
-      <c r="AH34" s="16"/>
-      <c r="AI34" s="16"/>
-      <c r="AJ34" s="16"/>
-      <c r="AK34" s="16"/>
-      <c r="AL34" s="16"/>
-      <c r="AM34" s="23"/>
-      <c r="AN34" s="23"/>
+      <c r="AE34" s="14"/>
+      <c r="AF34" s="14"/>
+      <c r="AG34" s="14"/>
+      <c r="AH34" s="14"/>
+      <c r="AI34" s="14"/>
+      <c r="AJ34" s="14"/>
+      <c r="AK34" s="14"/>
+      <c r="AL34" s="14"/>
+      <c r="AM34" s="20"/>
+      <c r="AN34" s="21"/>
     </row>
     <row r="35">
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C35" s="13">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F35" s="19">
+      <c r="F35" s="13">
         <v>33.0</v>
       </c>
-      <c r="G35" s="19">
+      <c r="G35" s="13">
         <v>32.0</v>
       </c>
-      <c r="H35" s="19" t="s">
+      <c r="H35" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="16"/>
-      <c r="T35" s="16"/>
-      <c r="U35" s="16"/>
-      <c r="V35" s="16"/>
-      <c r="W35" s="16"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="14"/>
+      <c r="W35" s="14"/>
       <c r="X35" s="15"/>
       <c r="Y35" s="15"/>
       <c r="Z35" s="15"/>
@@ -2979,167 +2944,167 @@
       <c r="AB35" s="15"/>
       <c r="AC35" s="15"/>
       <c r="AD35" s="15"/>
-      <c r="AE35" s="16"/>
-      <c r="AF35" s="16"/>
-      <c r="AG35" s="16"/>
-      <c r="AH35" s="16"/>
-      <c r="AI35" s="16"/>
-      <c r="AJ35" s="16"/>
-      <c r="AK35" s="16"/>
-      <c r="AL35" s="16"/>
-      <c r="AM35" s="24"/>
-      <c r="AN35" s="24"/>
+      <c r="AE35" s="14"/>
+      <c r="AF35" s="14"/>
+      <c r="AG35" s="14"/>
+      <c r="AH35" s="14"/>
+      <c r="AI35" s="14"/>
+      <c r="AJ35" s="14"/>
+      <c r="AK35" s="14"/>
+      <c r="AL35" s="14"/>
+      <c r="AM35" s="20"/>
+      <c r="AN35" s="21"/>
     </row>
     <row r="36">
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C36" s="13">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F36" s="19">
+      <c r="F36" s="13">
         <v>34.0</v>
       </c>
-      <c r="G36" s="19">
+      <c r="G36" s="13">
         <v>33.0</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H36" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="16"/>
-      <c r="N36" s="16"/>
-      <c r="O36" s="16"/>
-      <c r="P36" s="16"/>
-      <c r="Q36" s="16"/>
-      <c r="R36" s="16"/>
-      <c r="S36" s="16"/>
-      <c r="T36" s="16"/>
-      <c r="U36" s="16"/>
-      <c r="V36" s="16"/>
-      <c r="W36" s="16"/>
-      <c r="X36" s="22"/>
-      <c r="Y36" s="16"/>
-      <c r="Z36" s="16"/>
-      <c r="AA36" s="16"/>
-      <c r="AB36" s="16"/>
-      <c r="AC36" s="16"/>
-      <c r="AD36" s="16"/>
-      <c r="AE36" s="16"/>
-      <c r="AF36" s="16"/>
-      <c r="AG36" s="16"/>
-      <c r="AH36" s="16"/>
-      <c r="AI36" s="16"/>
-      <c r="AJ36" s="16"/>
-      <c r="AK36" s="16"/>
-      <c r="AL36" s="16"/>
-      <c r="AM36" s="16"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="14"/>
+      <c r="X36" s="19"/>
+      <c r="Y36" s="14"/>
+      <c r="Z36" s="14"/>
+      <c r="AA36" s="14"/>
+      <c r="AB36" s="14"/>
+      <c r="AC36" s="14"/>
+      <c r="AD36" s="14"/>
+      <c r="AE36" s="14"/>
+      <c r="AF36" s="14"/>
+      <c r="AG36" s="14"/>
+      <c r="AH36" s="14"/>
+      <c r="AI36" s="14"/>
+      <c r="AJ36" s="14"/>
+      <c r="AK36" s="14"/>
+      <c r="AL36" s="14"/>
+      <c r="AM36" s="14"/>
       <c r="AN36" s="16"/>
     </row>
     <row r="37">
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="12" t="s">
         <v>91</v>
       </c>
       <c r="C37" s="13">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="E37" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F37" s="13">
         <v>35.0</v>
       </c>
-      <c r="G37" s="19">
+      <c r="G37" s="13">
         <v>34.0</v>
       </c>
-      <c r="H37" s="19" t="s">
+      <c r="H37" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="16"/>
-      <c r="N37" s="16"/>
-      <c r="O37" s="16"/>
-      <c r="P37" s="16"/>
-      <c r="Q37" s="16"/>
-      <c r="R37" s="16"/>
-      <c r="S37" s="16"/>
-      <c r="T37" s="16"/>
-      <c r="U37" s="16"/>
-      <c r="V37" s="16"/>
-      <c r="W37" s="16"/>
-      <c r="X37" s="25"/>
-      <c r="Y37" s="16"/>
-      <c r="Z37" s="16"/>
-      <c r="AA37" s="16"/>
-      <c r="AB37" s="16"/>
-      <c r="AC37" s="16"/>
-      <c r="AD37" s="16"/>
-      <c r="AE37" s="16"/>
-      <c r="AF37" s="16"/>
-      <c r="AG37" s="16"/>
-      <c r="AH37" s="16"/>
-      <c r="AI37" s="16"/>
-      <c r="AJ37" s="16"/>
-      <c r="AK37" s="16"/>
-      <c r="AL37" s="16"/>
-      <c r="AM37" s="16"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="14"/>
+      <c r="X37" s="22"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="14"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="14"/>
+      <c r="AF37" s="14"/>
+      <c r="AG37" s="14"/>
+      <c r="AH37" s="14"/>
+      <c r="AI37" s="14"/>
+      <c r="AJ37" s="14"/>
+      <c r="AK37" s="14"/>
+      <c r="AL37" s="14"/>
+      <c r="AM37" s="14"/>
       <c r="AN37" s="16"/>
     </row>
     <row r="38">
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="12" t="s">
         <v>91</v>
       </c>
       <c r="C38" s="13">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F38" s="19">
+      <c r="F38" s="13">
         <v>36.0</v>
       </c>
-      <c r="G38" s="19">
+      <c r="G38" s="13">
         <v>35.0</v>
       </c>
-      <c r="H38" s="19" t="s">
+      <c r="H38" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="16"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="16"/>
-      <c r="O38" s="16"/>
-      <c r="P38" s="16"/>
-      <c r="Q38" s="16"/>
-      <c r="R38" s="16"/>
-      <c r="S38" s="16"/>
-      <c r="T38" s="16"/>
-      <c r="U38" s="16"/>
-      <c r="V38" s="16"/>
-      <c r="W38" s="16"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="14"/>
+      <c r="W38" s="14"/>
       <c r="X38" s="15"/>
       <c r="Y38" s="15"/>
       <c r="Z38" s="15"/>
@@ -3147,55 +3112,55 @@
       <c r="AB38" s="15"/>
       <c r="AC38" s="15"/>
       <c r="AD38" s="15"/>
-      <c r="AE38" s="16"/>
-      <c r="AF38" s="16"/>
-      <c r="AG38" s="16"/>
-      <c r="AH38" s="16"/>
-      <c r="AI38" s="16"/>
-      <c r="AJ38" s="16"/>
-      <c r="AK38" s="16"/>
-      <c r="AL38" s="16"/>
-      <c r="AM38" s="16"/>
+      <c r="AE38" s="14"/>
+      <c r="AF38" s="14"/>
+      <c r="AG38" s="14"/>
+      <c r="AH38" s="14"/>
+      <c r="AI38" s="14"/>
+      <c r="AJ38" s="14"/>
+      <c r="AK38" s="14"/>
+      <c r="AL38" s="14"/>
+      <c r="AM38" s="14"/>
       <c r="AN38" s="16"/>
     </row>
     <row r="39">
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C39" s="13">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F39" s="19">
+      <c r="F39" s="13">
         <v>37.0</v>
       </c>
-      <c r="G39" s="19" t="s">
+      <c r="G39" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="H39" s="19" t="s">
+      <c r="H39" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
-      <c r="N39" s="16"/>
-      <c r="O39" s="16"/>
-      <c r="P39" s="16"/>
-      <c r="Q39" s="16"/>
-      <c r="R39" s="16"/>
-      <c r="S39" s="16"/>
-      <c r="T39" s="16"/>
-      <c r="U39" s="16"/>
-      <c r="V39" s="16"/>
-      <c r="W39" s="16"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="14"/>
+      <c r="U39" s="14"/>
+      <c r="V39" s="14"/>
+      <c r="W39" s="14"/>
       <c r="X39" s="15"/>
       <c r="Y39" s="15"/>
       <c r="Z39" s="15"/>
@@ -3210,48 +3175,48 @@
       <c r="AI39" s="15"/>
       <c r="AJ39" s="15"/>
       <c r="AK39" s="15"/>
-      <c r="AL39" s="16"/>
-      <c r="AM39" s="16"/>
+      <c r="AL39" s="14"/>
+      <c r="AM39" s="14"/>
       <c r="AN39" s="16"/>
     </row>
     <row r="40">
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="12" t="s">
         <v>113</v>
       </c>
       <c r="C40" s="13">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F40" s="19">
+      <c r="F40" s="13">
         <v>24.0</v>
       </c>
-      <c r="G40" s="19">
+      <c r="G40" s="13">
         <v>40.0</v>
       </c>
-      <c r="H40" s="19" t="s">
+      <c r="H40" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I40" s="16"/>
-      <c r="J40" s="16"/>
-      <c r="K40" s="16"/>
-      <c r="L40" s="16"/>
-      <c r="M40" s="16"/>
-      <c r="N40" s="16"/>
-      <c r="O40" s="16"/>
-      <c r="P40" s="16"/>
-      <c r="Q40" s="16"/>
-      <c r="R40" s="16"/>
-      <c r="S40" s="16"/>
-      <c r="T40" s="16"/>
-      <c r="U40" s="16"/>
-      <c r="V40" s="16"/>
-      <c r="W40" s="16"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="14"/>
       <c r="X40" s="15"/>
       <c r="Y40" s="15"/>
       <c r="Z40" s="15"/>
@@ -3271,43 +3236,43 @@
       <c r="AN40" s="16"/>
     </row>
     <row r="41">
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="12" t="s">
         <v>113</v>
       </c>
       <c r="C41" s="13">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F41" s="19">
+      <c r="F41" s="13">
         <v>24.0</v>
       </c>
-      <c r="G41" s="19">
+      <c r="G41" s="13">
         <v>40.0</v>
       </c>
-      <c r="H41" s="19" t="s">
+      <c r="H41" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="16"/>
-      <c r="N41" s="16"/>
-      <c r="O41" s="16"/>
-      <c r="P41" s="16"/>
-      <c r="Q41" s="16"/>
-      <c r="R41" s="16"/>
-      <c r="S41" s="16"/>
-      <c r="T41" s="16"/>
-      <c r="U41" s="16"/>
-      <c r="V41" s="16"/>
-      <c r="W41" s="16"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="14"/>
+      <c r="U41" s="14"/>
+      <c r="V41" s="14"/>
+      <c r="W41" s="14"/>
       <c r="X41" s="15"/>
       <c r="Y41" s="15"/>
       <c r="Z41" s="15"/>
@@ -3327,43 +3292,43 @@
       <c r="AN41" s="16"/>
     </row>
     <row r="42">
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="12" t="s">
         <v>113</v>
       </c>
       <c r="C42" s="13">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="19">
+      <c r="F42" s="13">
         <v>24.0</v>
       </c>
-      <c r="G42" s="19">
+      <c r="G42" s="13">
         <v>40.0</v>
       </c>
-      <c r="H42" s="19" t="s">
+      <c r="H42" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I42" s="16"/>
+      <c r="I42" s="14"/>
       <c r="J42" s="14"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="16"/>
-      <c r="M42" s="16"/>
-      <c r="N42" s="16"/>
-      <c r="O42" s="16"/>
-      <c r="P42" s="16"/>
-      <c r="Q42" s="16"/>
-      <c r="R42" s="16"/>
-      <c r="S42" s="16"/>
-      <c r="T42" s="16"/>
-      <c r="U42" s="16"/>
-      <c r="V42" s="16"/>
-      <c r="W42" s="16"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
       <c r="X42" s="15"/>
       <c r="Y42" s="15"/>
       <c r="Z42" s="15"/>
@@ -3383,30 +3348,30 @@
       <c r="AN42" s="16"/>
     </row>
     <row r="43">
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C43" s="13">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E43" s="19" t="s">
+      <c r="E43" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F43" s="19" t="s">
+      <c r="F43" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G43" s="19">
+      <c r="G43" s="13">
         <v>41.0</v>
       </c>
-      <c r="H43" s="19" t="s">
+      <c r="H43" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I43" s="16"/>
-      <c r="J43" s="16"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
@@ -3417,98 +3382,98 @@
       <c r="R43" s="15"/>
       <c r="S43" s="15"/>
       <c r="T43" s="15"/>
-      <c r="U43" s="16"/>
-      <c r="V43" s="16"/>
-      <c r="W43" s="16"/>
-      <c r="X43" s="16"/>
-      <c r="Y43" s="16"/>
-      <c r="Z43" s="16"/>
-      <c r="AA43" s="16"/>
-      <c r="AB43" s="16"/>
-      <c r="AC43" s="16"/>
-      <c r="AD43" s="16"/>
-      <c r="AE43" s="16"/>
-      <c r="AF43" s="16"/>
-      <c r="AG43" s="16"/>
-      <c r="AH43" s="16"/>
-      <c r="AI43" s="16"/>
-      <c r="AJ43" s="16"/>
-      <c r="AK43" s="16"/>
-      <c r="AL43" s="16"/>
-      <c r="AM43" s="16"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="14"/>
+      <c r="W43" s="14"/>
+      <c r="X43" s="14"/>
+      <c r="Y43" s="14"/>
+      <c r="Z43" s="14"/>
+      <c r="AA43" s="14"/>
+      <c r="AB43" s="14"/>
+      <c r="AC43" s="14"/>
+      <c r="AD43" s="14"/>
+      <c r="AE43" s="14"/>
+      <c r="AF43" s="14"/>
+      <c r="AG43" s="14"/>
+      <c r="AH43" s="14"/>
+      <c r="AI43" s="14"/>
+      <c r="AJ43" s="14"/>
+      <c r="AK43" s="14"/>
+      <c r="AL43" s="14"/>
+      <c r="AM43" s="14"/>
       <c r="AN43" s="16"/>
     </row>
     <row r="44">
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="C44" s="13">
+      <c r="C44" s="24">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="D44" s="27" t="s">
+      <c r="D44" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="E44" s="27" t="s">
+      <c r="E44" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="27">
+      <c r="F44" s="24">
         <v>40.0</v>
       </c>
-      <c r="G44" s="27" t="s">
+      <c r="G44" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="H44" s="27" t="s">
+      <c r="H44" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="I44" s="28"/>
-      <c r="J44" s="28"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
-      <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="15"/>
-      <c r="AA44" s="15"/>
-      <c r="AB44" s="15"/>
-      <c r="AC44" s="15"/>
-      <c r="AD44" s="15"/>
-      <c r="AE44" s="15"/>
-      <c r="AF44" s="15"/>
-      <c r="AG44" s="15"/>
-      <c r="AH44" s="15"/>
-      <c r="AI44" s="15"/>
-      <c r="AJ44" s="15"/>
-      <c r="AK44" s="15"/>
-      <c r="AL44" s="15"/>
-      <c r="AM44" s="15"/>
-      <c r="AN44" s="16"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="26"/>
+      <c r="N44" s="26"/>
+      <c r="O44" s="26"/>
+      <c r="P44" s="26"/>
+      <c r="Q44" s="26"/>
+      <c r="R44" s="26"/>
+      <c r="S44" s="26"/>
+      <c r="T44" s="26"/>
+      <c r="U44" s="26"/>
+      <c r="V44" s="26"/>
+      <c r="W44" s="26"/>
+      <c r="X44" s="26"/>
+      <c r="Y44" s="26"/>
+      <c r="Z44" s="26"/>
+      <c r="AA44" s="26"/>
+      <c r="AB44" s="26"/>
+      <c r="AC44" s="26"/>
+      <c r="AD44" s="26"/>
+      <c r="AE44" s="26"/>
+      <c r="AF44" s="26"/>
+      <c r="AG44" s="26"/>
+      <c r="AH44" s="26"/>
+      <c r="AI44" s="26"/>
+      <c r="AJ44" s="26"/>
+      <c r="AK44" s="26"/>
+      <c r="AL44" s="26"/>
+      <c r="AM44" s="26"/>
+      <c r="AN44" s="27"/>
     </row>
     <row r="46">
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="I46" s="29" t="s">
+      <c r="I46" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="J46" s="29" t="s">
+      <c r="J46" s="28" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="47">
-      <c r="H47" s="15"/>
+      <c r="H47" s="29"/>
       <c r="I47" s="30"/>
-      <c r="J47" s="25"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>